<commit_message>
point spoken language expression observation to the correct value set
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-splasch-SpokenLanguageExpressionObservation.xlsx
+++ b/output/StructureDefinition-splasch-SpokenLanguageExpressionObservation.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2021-12-09T02:52:24-05:00</t>
+    <t>2021-12-10T12:07:05-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -676,7 +676,7 @@
     <t>Knowing what kind of observation is being made is essential to understanding the observation.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/pacio-splasch/ValueSet/SPLASCHSpeechComprehensionObservationVS</t>
+    <t>http://hl7.org/fhir/us/pacio-splasch/ValueSet/SPLASCHSpeechExpressionObservationVS</t>
   </si>
   <si>
     <t>Event.code</t>
@@ -1807,7 +1807,7 @@
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="60.515625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="84.40234375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="79.79296875" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="23.8515625" customWidth="true" bestFit="true"/>

</xml_diff>